<commit_message>
cambie los nombres de los excel,empleados ahora solo funciona con 1 excel, verificar busca en clientes y empleados, las funciones de los empleados ya estan en la barra de menus y falta la opcion para cambio de pin
</commit_message>
<xml_diff>
--- a/empleados.xlsx
+++ b/empleados.xlsx
@@ -15,21 +15,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>carlos</t>
-  </si>
-  <si>
-    <t>sss</t>
-  </si>
-  <si>
-    <t>cesar</t>
-  </si>
-  <si>
-    <t>Karina</t>
-  </si>
-  <si>
-    <t>2233</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>Cesar</t>
+  </si>
+  <si>
+    <t>2222</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -386,56 +389,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="n">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
-        <v>121212</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>21212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="n">
-        <v>1234</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="n">
-        <v>1022</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
         <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>